<commit_message>
Python Code to encode data test
Created python file to encode data, tested with sex feature.
Works with sex feature, need to copy over other features
</commit_message>
<xml_diff>
--- a/Other dataset/Other Dataset/Ordinal encoding.xlsx
+++ b/Other dataset/Other Dataset/Ordinal encoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\Year 4 work\Applied-Data-Science-Coursework\Applied-Data-Science-Coursework\Other dataset\Other Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2A8EF4-FA2C-4A66-A90E-F7A715C62F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0E74E-05E2-4403-845E-48ED60E557FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>All NaNs/missing answers are encoded as 0</t>
-  </si>
-  <si>
     <t>LikeMusic7</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>DepressionTeach7</t>
+  </si>
+  <si>
+    <t>All NaNs/missing answers are encoded as NaN</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D209" sqref="D209"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,10 +753,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -807,10 +807,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
         <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -961,10 +961,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
         <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -988,10 +988,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1069,10 +1069,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1096,10 +1096,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -1150,10 +1150,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
         <v>33</v>
-      </c>
-      <c r="B57" t="s">
-        <v>34</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -1296,10 +1296,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" t="s">
         <v>39</v>
-      </c>
-      <c r="B64" t="s">
-        <v>40</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C66">
         <v>3</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67">
         <v>4</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C68">
         <v>5</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C69">
         <v>6</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C70">
         <v>7</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C71">
         <v>8</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C75">
         <v>4</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C76">
         <v>5</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C77">
         <v>6</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C78">
         <v>7</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C85">
         <v>5</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C86">
         <v>6</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C87">
         <v>7</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C88">
         <v>8</v>
@@ -1508,10 +1508,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C90">
         <v>2</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C91">
         <v>3</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C92">
         <v>4</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C94">
         <v>6</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C95">
         <v>7</v>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B96" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B98" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B100" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C101">
         <v>2</v>
@@ -1624,10 +1624,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C103">
         <v>2</v>
@@ -1643,10 +1643,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>54</v>
+      </c>
+      <c r="B104" t="s">
         <v>55</v>
-      </c>
-      <c r="B104" t="s">
-        <v>56</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C107">
         <v>4</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C108">
         <v>5</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C109">
         <v>6</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C110">
         <v>7</v>
@@ -1702,10 +1702,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B111" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C113">
         <v>3</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C114">
         <v>4</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C115">
         <v>5</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C116">
         <v>6</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C117">
         <v>7</v>
@@ -1761,10 +1761,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B118" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C121">
         <v>2</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C122">
         <v>3</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C123">
         <v>4</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C124">
         <v>5</v>
@@ -1823,10 +1823,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B125" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C126">
         <v>2</v>
@@ -1842,10 +1842,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B127" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C128">
         <v>2</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C130">
         <v>2</v>
@@ -1880,10 +1880,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B131" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C132">
         <v>2</v>
@@ -1899,10 +1899,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B133" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C134">
         <v>2</v>
@@ -1918,10 +1918,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B135" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C136">
         <v>2</v>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B137" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C138">
         <v>2</v>
@@ -1956,10 +1956,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>72</v>
+      </c>
+      <c r="B139" t="s">
         <v>73</v>
-      </c>
-      <c r="B139" t="s">
-        <v>74</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C140">
         <v>2</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C141">
         <v>3</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C142">
         <v>4</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C143">
         <v>5</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C144">
         <v>6</v>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>79</v>
+      </c>
+      <c r="B145" t="s">
         <v>80</v>
-      </c>
-      <c r="B145" t="s">
-        <v>81</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C146">
         <v>2</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C147">
         <v>3</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C148">
         <v>4</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C150">
         <v>6</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C151">
         <v>7</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C152">
         <v>8</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C153">
         <v>9</v>
@@ -2082,10 +2082,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B154" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C155">
         <v>2</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C156">
         <v>3</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C157">
         <v>4</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C158">
         <v>5</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C159">
         <v>6</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C160">
         <v>7</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C161">
         <v>8</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C162">
         <v>9</v>
@@ -2157,10 +2157,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B163" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C164">
         <v>2</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C165">
         <v>3</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C166">
         <v>4</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C167">
         <v>5</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C168">
         <v>6</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C169">
         <v>7</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C170">
         <v>8</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C171">
         <v>9</v>
@@ -2232,10 +2232,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>91</v>
+      </c>
+      <c r="B172" t="s">
         <v>92</v>
-      </c>
-      <c r="B172" t="s">
-        <v>93</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C173">
         <v>2</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C174">
         <v>3</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C175">
         <v>4</v>
@@ -2267,10 +2267,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>96</v>
+      </c>
+      <c r="B176" t="s">
         <v>97</v>
-      </c>
-      <c r="B176" t="s">
-        <v>98</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C178">
         <v>3</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C179">
         <v>4</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C180">
         <v>5</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C181">
         <v>6</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B182" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C183">
         <v>2</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C184">
         <v>3</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C185">
         <v>4</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C186">
         <v>5</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C187">
         <v>6</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C188">
         <v>7</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C189">
         <v>8</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C190">
         <v>9</v>
@@ -2393,10 +2393,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>109</v>
+      </c>
+      <c r="B191" t="s">
         <v>110</v>
-      </c>
-      <c r="B191" t="s">
-        <v>111</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C192">
         <v>2</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C193">
         <v>3</v>
@@ -2420,10 +2420,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B194" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C195">
         <v>2</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C196">
         <v>3</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B197" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C198">
         <v>2</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C199">
         <v>3</v>
@@ -2474,10 +2474,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B200" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C201">
         <v>2</v>
@@ -2493,5 +2493,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>